<commit_message>
Added Category Parent ID
</commit_message>
<xml_diff>
--- a/public/categoryParent.xlsx
+++ b/public/categoryParent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/islam.eddassouli/Desktop/VercelHomepageAPP/app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0926EC2-9BF2-C241-8D3D-7AB34AB189C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F329F06-80D2-6844-84A8-E6BAB1412F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30240" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="585">
   <si>
     <t>Category ID</t>
   </si>
@@ -1710,6 +1710,84 @@
   </si>
   <si>
     <t>Co-ords</t>
+  </si>
+  <si>
+    <t>men-642</t>
+  </si>
+  <si>
+    <t>men-642-twin-pack</t>
+  </si>
+  <si>
+    <t>men-big-brother</t>
+  </si>
+  <si>
+    <t>men-big-jean</t>
+  </si>
+  <si>
+    <t>men-bob</t>
+  </si>
+  <si>
+    <t>men-bro</t>
+  </si>
+  <si>
+    <t>men-combat</t>
+  </si>
+  <si>
+    <t>men-cool-guy</t>
+  </si>
+  <si>
+    <t>men-eros</t>
+  </si>
+  <si>
+    <t>men-richard</t>
+  </si>
+  <si>
+    <t>men-sexy-twist</t>
+  </si>
+  <si>
+    <t>men-skater</t>
+  </si>
+  <si>
+    <t>men-super-twinky</t>
+  </si>
+  <si>
+    <t>men-tidy-biker</t>
+  </si>
+  <si>
+    <t>women-642</t>
+  </si>
+  <si>
+    <t>women-80s</t>
+  </si>
+  <si>
+    <t>women-boston</t>
+  </si>
+  <si>
+    <t>women-capri</t>
+  </si>
+  <si>
+    <t>women-cool-girl</t>
+  </si>
+  <si>
+    <t>women-eros</t>
+  </si>
+  <si>
+    <t>women-flare</t>
+  </si>
+  <si>
+    <t>women-jennifer</t>
+  </si>
+  <si>
+    <t>women-roadie</t>
+  </si>
+  <si>
+    <t>women-traveller</t>
+  </si>
+  <si>
+    <t>women--trumpet</t>
+  </si>
+  <si>
+    <t>women-twiggy</t>
   </si>
 </sst>
 </file>
@@ -1987,10 +2065,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:B999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A529" workbookViewId="0">
-      <selection activeCell="G541" sqref="G541"/>
+    <sheetView tabSelected="1" topLeftCell="A559" workbookViewId="0">
+      <selection activeCell="D585" sqref="D585"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6504,108 +6582,212 @@
       </c>
     </row>
     <row r="564" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A564" s="3"/>
-      <c r="B564" s="2"/>
+      <c r="A564" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="B564" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="565" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A565" s="2"/>
-      <c r="B565" s="2"/>
+      <c r="A565" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B565" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="566" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A566" s="2"/>
-      <c r="B566" s="2"/>
+      <c r="A566" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B566" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="567" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A567" s="2"/>
-      <c r="B567" s="2"/>
+      <c r="A567" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B567" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="568" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A568" s="2"/>
-      <c r="B568" s="2"/>
+      <c r="A568" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B568" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="569" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A569" s="2"/>
-      <c r="B569" s="2"/>
+      <c r="A569" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B569" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="570" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A570" s="2"/>
-      <c r="B570" s="2"/>
+      <c r="A570" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B570" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="571" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A571" s="2"/>
-      <c r="B571" s="2"/>
+      <c r="A571" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B571" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="572" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A572" s="2"/>
-      <c r="B572" s="2"/>
+      <c r="A572" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B572" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="573" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A573" s="2"/>
-      <c r="B573" s="2"/>
+      <c r="A573" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B573" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="574" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A574" s="2"/>
-      <c r="B574" s="2"/>
+      <c r="A574" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B574" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="575" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A575" s="2"/>
-      <c r="B575" s="2"/>
+      <c r="A575" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B575" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="576" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A576" s="2"/>
-      <c r="B576" s="2"/>
+      <c r="A576" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B576" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="577" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A577" s="2"/>
-      <c r="B577" s="2"/>
+      <c r="A577" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B577" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="578" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A578" s="2"/>
-      <c r="B578" s="2"/>
+      <c r="A578" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B578" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="579" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A579" s="2"/>
-      <c r="B579" s="2"/>
+      <c r="A579" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B579" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="580" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A580" s="2"/>
-      <c r="B580" s="2"/>
+      <c r="A580" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B580" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="581" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A581" s="2"/>
-      <c r="B581" s="2"/>
+      <c r="A581" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="B581" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="582" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A582" s="2"/>
-      <c r="B582" s="2"/>
+      <c r="A582" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B582" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="583" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A583" s="2"/>
-      <c r="B583" s="2"/>
+      <c r="A583" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B583" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="584" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A584" s="2"/>
-      <c r="B584" s="2"/>
+      <c r="A584" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="B584" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="585" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A585" s="2"/>
-      <c r="B585" s="2"/>
+      <c r="A585" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B585" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="586" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A586" s="2"/>
-      <c r="B586" s="2"/>
+      <c r="A586" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B586" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="587" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A587" s="2"/>
-      <c r="B587" s="2"/>
+      <c r="A587" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="B587" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="588" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A588" s="2"/>
-      <c r="B588" s="2"/>
+      <c r="A588" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B588" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="589" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A589" s="2"/>
-      <c r="B589" s="2"/>
+      <c r="A589" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B589" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="590" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A590" s="2"/>
@@ -8246,10 +8428,6 @@
     <row r="999" spans="1:2" ht="13" x14ac:dyDescent="0.15">
       <c r="A999" s="2"/>
       <c r="B999" s="2"/>
-    </row>
-    <row r="1000" spans="1:2" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>